<commit_message>
new push on 18/03/2025
</commit_message>
<xml_diff>
--- a/OnlineMarriageSystem/TestData/matrimony.xlsx
+++ b/OnlineMarriageSystem/TestData/matrimony.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranja\source\repos\OnlineMarriageSystem\OnlineMarriageSystem\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C35EE68-595E-4988-88D3-48AACD7C927C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="7200" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Husb" sheetId="1" r:id="rId1"/>
     <sheet name="wife" sheetId="2" r:id="rId2"/>
     <sheet name="wittness" sheetId="3" r:id="rId3"/>
+    <sheet name="ReportDate" sheetId="4" r:id="rId4"/>
+    <sheet name="RegNumToSearch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>DateMa</t>
   </si>
@@ -102,18 +105,33 @@
   <si>
     <t>kaka3</t>
   </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>regno</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF737C85"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,9 +154,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +437,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -489,7 +508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -561,10 +580,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -613,4 +632,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557D18F2-10A0-4918-A052-141D770DD430}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1">
+        <v>38809</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>38870</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB6161B-62CE-4F90-8B07-46B5F492087C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2">
+        <v>290346708</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>